<commit_message>
Updated doc with info from the new card
</commit_message>
<xml_diff>
--- a/Documentation/Stats of components.xlsx
+++ b/Documentation/Stats of components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flavie\Documents\FixedChallenge2019_Elec\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FED5EAF-094B-48FF-95E6-1E0E38A9804B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DADB2E2-D591-42F5-8EB2-E0C3833969F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{98EE39C2-5162-4388-BADD-6D8C615B5862}"/>
   </bookViews>
@@ -1460,6 +1460,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -1888,6 +1895,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -3269,8 +3283,8 @@
     <tableColumn id="2" xr3:uid="{A8E1287F-8F36-4670-86E5-AC80751EDBBA}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{43C3BA04-61B5-4174-BB9C-BAA4AB56B3E0}" uniqueName="3" name="Pattern" queryTableFieldId="3" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{4E7F9E91-2D33-4679-B5C6-9EEB8A1ACA01}" uniqueName="4" name="Quantity" queryTableFieldId="4"/>
-    <tableColumn id="7" xr3:uid="{4EDF46C9-98D1-47BF-96CB-04156AEB0361}" uniqueName="7" name="$/u" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{D339491B-CEB7-49EC-A3CC-4D67843A4285}" uniqueName="8" name="Total $" queryTableFieldId="8" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{4EDF46C9-98D1-47BF-96CB-04156AEB0361}" uniqueName="7" name="$/u" queryTableFieldId="7" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{D339491B-CEB7-49EC-A3CC-4D67843A4285}" uniqueName="8" name="Total $" queryTableFieldId="8" dataDxfId="10">
       <calculatedColumnFormula>bom__3[[#This Row],[$/u]]*bom__3[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3282,12 +3296,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{19B7E748-EF1B-4843-A376-3B363223FC37}" name="bom__2" displayName="bom__2" ref="A1:F48" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F48" xr:uid="{478A3E03-C2DD-4A1E-ABA5-75641B448821}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A2DD74E9-6568-4677-B9BF-D04AE88F99E2}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{249599F9-81FC-4B33-8A23-3F79D9406310}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{11E58577-3254-4FC3-A945-76B2B30C8082}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{A2DD74E9-6568-4677-B9BF-D04AE88F99E2}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{249599F9-81FC-4B33-8A23-3F79D9406310}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{11E58577-3254-4FC3-A945-76B2B30C8082}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{9266E48F-D770-49AB-A529-8D04676BE8D8}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{164E71C2-95CE-4B38-9015-0F5F6509E4D5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{F735E32C-AB16-479B-AE77-7F3A39333300}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{164E71C2-95CE-4B38-9015-0F5F6509E4D5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{F735E32C-AB16-479B-AE77-7F3A39333300}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3297,12 +3311,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38A10EAE-7A50-4157-9ED6-2E593FABFA47}" name="bom" displayName="bom" ref="A1:F49" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:F49" xr:uid="{A3138735-CA50-4B1A-8499-84D95BB070BA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FAC1206A-E05A-4A74-B900-4D7E8196A4BD}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{228D5F73-8BF9-4BAF-AB16-2F2F4683D24F}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{7015CCCF-A163-4986-ACDC-2CF23B5F97F9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{FAC1206A-E05A-4A74-B900-4D7E8196A4BD}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{228D5F73-8BF9-4BAF-AB16-2F2F4683D24F}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{7015CCCF-A163-4986-ACDC-2CF23B5F97F9}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{CE09CE91-5D59-462A-856B-A07271E18CEE}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{AA664769-C7CE-4B2B-AF19-5D1024726FB7}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{8BFD148C-F3CC-4796-8930-3E3578D414E6}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{AA664769-C7CE-4B2B-AF19-5D1024726FB7}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{8BFD148C-F3CC-4796-8930-3E3578D414E6}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3607,16 +3621,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169B82B1-A0E5-4871-8A39-98A5D0E95F13}">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="26" zoomScaleNormal="26" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.90625" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>